<commit_message>
Saving Data in Excel too
</commit_message>
<xml_diff>
--- a/TCCWEBAPP/TCC.xlsx
+++ b/TCCWEBAPP/TCC.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,6 +412,18 @@
       <c r="C1" t="str">
         <v>Year</v>
       </c>
+      <c r="D1" t="str">
+        <v>Outcome Of Case</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Type of Issue</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Gender of Appellant</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Gender of Judge</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -423,6 +435,18 @@
       <c r="C2" t="str">
         <v>2003</v>
       </c>
+      <c r="D2" t="str">
+        <v>Losing</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Income Tax</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Female</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Female</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -434,6 +458,18 @@
       <c r="C3" t="str">
         <v>2003</v>
       </c>
+      <c r="D3" t="str">
+        <v>Losing</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Employment Insurance Act</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Male</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Male</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -445,6 +481,18 @@
       <c r="C4" t="str">
         <v>2003</v>
       </c>
+      <c r="D4" t="str">
+        <v>Losing</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Income Tax</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Male</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Male</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -470,7 +518,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved the Chunk Problem for Large text Input and Also added a file for the NLP Text Summaraization Problem
</commit_message>
<xml_diff>
--- a/TCCWEBAPP/TCC.xlsx
+++ b/TCCWEBAPP/TCC.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,10 +419,22 @@
         <v>Type of Issue</v>
       </c>
       <c r="F1" t="str">
+        <v>Inital Comparison</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Duration of the Case</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Type of Tax Payer</v>
+      </c>
+      <c r="I1" t="str">
         <v>Gender of Appellant</v>
       </c>
-      <c r="G1" t="str">
+      <c r="J1" t="str">
         <v>Gender of Judge</v>
+      </c>
+      <c r="K1" t="str">
+        <v>URL</v>
       </c>
     </row>
     <row r="2">
@@ -441,108 +453,125 @@
       <c r="E2" t="str">
         <v>Income Tax</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="str">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Individual</v>
+      </c>
+      <c r="I2" t="str">
         <v>Female</v>
       </c>
-      <c r="G2" t="str">
+      <c r="J2" t="str">
         <v>Female</v>
+      </c>
+      <c r="K2" t="str">
+        <f>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26605/index.do</f>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26815/index.do</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> D.W. Beaubier</v>
+        <v>D.G.H. Bowman</v>
       </c>
       <c r="B3" t="str">
-        <v>CHARLES W. DOERING,</v>
+        <v>CHARLES B. LOEWEN,</v>
       </c>
       <c r="C3" t="str">
         <v>2003</v>
       </c>
       <c r="D3" t="str">
-        <v>Losing</v>
+        <v>Partially Winning</v>
       </c>
       <c r="E3" t="str">
-        <v>Employment Insurance Act</v>
-      </c>
-      <c r="F3" t="str">
+        <v>Income Tax</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Individual</v>
+      </c>
+      <c r="I3" t="str">
         <v>Male</v>
       </c>
-      <c r="G3" t="str">
+      <c r="J3" t="str">
         <v>Male</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>C.H. McArthur</v>
+        <v xml:space="preserve"> D.W. Beaubier</v>
       </c>
       <c r="B4" t="str">
-        <v>MICHAEL LAURIE,</v>
+        <v>DOUGLAS DIXON,</v>
       </c>
       <c r="C4" t="str">
         <v>2003</v>
       </c>
       <c r="D4" t="str">
-        <v>Losing</v>
+        <v>Partially Winning</v>
       </c>
       <c r="E4" t="str">
-        <v>Income tax</v>
-      </c>
-      <c r="F4" t="str">
+        <v>Income Tax</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Less than 1 year</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Partnership</v>
+      </c>
+      <c r="I4" t="str">
         <v>Male</v>
       </c>
-      <c r="G4" t="str">
+      <c r="J4" t="str">
         <v>Male</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v xml:space="preserve"> D.W. Beaubier</v>
+        <v xml:space="preserve"> Diane Campbell</v>
       </c>
       <c r="B5" t="str">
-        <v>DOUGLAS DIXON,</v>
+        <v>S.K. MANAGEMENT INC.,&amp;&amp;&amp;#CORPORATION</v>
       </c>
       <c r="C5" t="str">
         <v>2003</v>
       </c>
       <c r="D5" t="str">
-        <v>Partially Winning</v>
+        <v>Losing</v>
       </c>
       <c r="E5" t="str">
-        <v>Income Tax</v>
-      </c>
-      <c r="F5" t="str">
+        <v>Excise tax</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Less than 1 year</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Corporation</v>
+      </c>
+      <c r="I5" t="str">
         <v>Male</v>
       </c>
-      <c r="G5" t="str">
-        <v>Male</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>A.A. Sarchuk</v>
-      </c>
-      <c r="B6" t="str">
-        <v>HONORA ZAKRISON,</v>
-      </c>
-      <c r="C6" t="str">
-        <v>2003</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Losing</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Income Tax</v>
-      </c>
-      <c r="F6" t="str">
+      <c r="J5" t="str">
         <v>Female</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Male</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gpt model Updated and Large input text handled
</commit_message>
<xml_diff>
--- a/TCCWEBAPP/TCC.xlsx
+++ b/TCCWEBAPP/TCC.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,30 +419,36 @@
         <v>Type of Issue</v>
       </c>
       <c r="F1" t="str">
+        <v>Intial of Appellant</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Intital of Judge</v>
+      </c>
+      <c r="H1" t="str">
         <v>Inital Comparison</v>
       </c>
-      <c r="G1" t="str">
+      <c r="I1" t="str">
         <v>Duration of the Case</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>Type of Tax Payer</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>Gender of Appellant</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>Gender of Judge</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>URL</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve"> Lucie Lamarre</v>
+        <v xml:space="preserve"> D.W. Rowe</v>
       </c>
       <c r="B2" t="str">
-        <v>MANON RODIER,</v>
+        <v>GORDON LAWRENCE SCOTT,</v>
       </c>
       <c r="C2" t="str">
         <v>2003</v>
@@ -451,100 +457,159 @@
         <v>Losing</v>
       </c>
       <c r="E2" t="str">
-        <v>Income Tax</v>
-      </c>
-      <c r="F2">
+        <v>Income tax</v>
+      </c>
+      <c r="F2" t="str">
+        <v>G.L.S.</v>
+      </c>
+      <c r="G2" t="str">
+        <v>D.W.R.</v>
+      </c>
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="G2" t="str">
-        <v>Less than 1 year</v>
-      </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
+        <v>5</v>
+      </c>
+      <c r="J2" t="str">
         <v>Individual</v>
       </c>
-      <c r="I2" t="str">
-        <v>Female</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Female</v>
-      </c>
       <c r="K2" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26815/index.do</v>
+        <v>Male</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Male</v>
+      </c>
+      <c r="M2" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26824/index.do</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> D.W. Beaubier</v>
+        <v xml:space="preserve"> Pierre Archambault</v>
       </c>
       <c r="B3" t="str">
-        <v>CHARLES W. DOERING,</v>
+        <v>RONA INC.&amp;&amp;&amp;#CORPORATION</v>
       </c>
       <c r="C3" t="str">
         <v>2003</v>
       </c>
       <c r="D3" t="str">
-        <v>Losing</v>
+        <v>Partially Winning</v>
       </c>
       <c r="E3" t="str">
-        <v>Employment Insurance Act</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
+        <v>Income Tax Act</v>
+      </c>
+      <c r="F3" t="str">
+        <v>RI</v>
       </c>
       <c r="G3" t="str">
-        <v>2</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Individual</v>
+        <v>PA</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
       </c>
       <c r="I3" t="str">
+        <v>2000-2003 (3 years)</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Corporation</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="L3" t="str">
         <v>Male</v>
       </c>
-      <c r="J3" t="str">
-        <v>Male</v>
-      </c>
-      <c r="K3" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/27929/index.do</v>
+      <c r="M3" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26816/index.do</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>D.G.H. Bowman</v>
+        <v xml:space="preserve"> R.D. Bell</v>
       </c>
       <c r="B4" t="str">
-        <v>CHARLES B. LOEWEN,</v>
+        <v>DALE COLBRAN,</v>
       </c>
       <c r="C4" t="str">
         <v>2003</v>
       </c>
       <c r="D4" t="str">
+        <v>Winning</v>
+      </c>
+      <c r="E4" t="str">
+        <v>GST</v>
+      </c>
+      <c r="F4" t="str">
+        <v>D.C.</v>
+      </c>
+      <c r="G4" t="str">
+        <v>R.D.B.</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4" t="str">
+        <v>3</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Individual</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Male</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Male</v>
+      </c>
+      <c r="M4" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26094/index.do</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B5" t="str">
+        <v>GUYLAINE DUCHAINE,</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2003</v>
+      </c>
+      <c r="D5" t="str">
         <v>Partially Winning</v>
       </c>
-      <c r="E4" t="str">
-        <v>Income Tax</v>
-      </c>
-      <c r="F4">
+      <c r="E5" t="str">
+        <v>Income Tax Act</v>
+      </c>
+      <c r="F5" t="str">
+        <v>GD</v>
+      </c>
+      <c r="G5" t="str">
+        <v>FA</v>
+      </c>
+      <c r="H5">
         <v>6</v>
       </c>
-      <c r="G4" t="str">
-        <v>2</v>
-      </c>
-      <c r="H4" t="str">
+      <c r="I5" t="str">
+        <v>2003-1999=4 years</v>
+      </c>
+      <c r="J5" t="str">
         <v>Individual</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K5" t="str">
+        <v>Female</v>
+      </c>
+      <c r="L5" t="str">
         <v>Male</v>
       </c>
-      <c r="J4" t="str">
-        <v>Male</v>
-      </c>
-      <c r="K4" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26605/index.do</v>
+      <c r="M5" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/26977/index.do</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Result JSON folder has all Json data from API
</commit_message>
<xml_diff>
--- a/TCCWEBAPP/TCC.xlsx
+++ b/TCCWEBAPP/TCC.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,324 +445,324 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> Valerie Miller</v>
       </c>
       <c r="B2" t="str">
-        <v>LIN L. KEEHN,</v>
+        <v>RANDY J. OLLENBERGER,</v>
       </c>
       <c r="C2" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M2" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521038/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30857/index.do</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> Réal Favreau</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B3" t="str">
-        <v>POLARSAT INC.,</v>
+        <v>MARIA LUCARELLI,</v>
       </c>
       <c r="C3" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M3" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521044/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30931/index.do</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> Robert J. Hogan</v>
       </c>
       <c r="B4" t="str">
-        <v>MICHAEL GREER,</v>
+        <v>JAGMOHAN SINGH GILL,</v>
       </c>
       <c r="C4" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M4" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521125/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30946/index.do</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Eugene P. Rossiter</v>
+        <v xml:space="preserve"> Lucie Lamarre</v>
       </c>
       <c r="B5" t="str">
-        <v>NAVDEEP SINDHI,</v>
+        <v>ANNITA EMOND,</v>
       </c>
       <c r="C5" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M5" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521126/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30933/index.do</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v xml:space="preserve"> Gabrielle St-Hilaire</v>
+        <v xml:space="preserve"> Patrick Boyle</v>
       </c>
       <c r="B6" t="str">
-        <v>MOHAMMAD YADGAR,</v>
+        <v>GROUPE HONCO INC.,</v>
       </c>
       <c r="C6" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M6" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521127/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30940/index.do</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v xml:space="preserve"> Ronald MacPhee</v>
+        <v xml:space="preserve"> J.E. Hershfield</v>
       </c>
       <c r="B7" t="str">
-        <v>MIRIAM WATTS,</v>
+        <v>JI-HWAN PARK,</v>
       </c>
       <c r="C7" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M7" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521056/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30935/index.do</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Justice Gaston Jorré</v>
+        <v xml:space="preserve"> Robert J. Hogan</v>
       </c>
       <c r="B8" t="str">
-        <v>2489869 ONTARIO INC.,</v>
+        <v>DEBORAH MAASS-HOWARD,</v>
       </c>
       <c r="C8" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M8" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521051/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31004/index.do</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v xml:space="preserve"> Réal Favreau</v>
+        <v xml:space="preserve"> J.E. Hershfield</v>
       </c>
       <c r="B9" t="str">
-        <v>JOHN MICHALUK,</v>
+        <v>763993 ALBERTA LTD.,</v>
       </c>
       <c r="C9" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M9" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521043/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30936/index.do</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v xml:space="preserve">JudgeName Not Found in Pattern also </v>
+        <v xml:space="preserve"> Réal Favreau</v>
       </c>
       <c r="B10" t="str">
-        <v>BRANDON OSADCHUCK,</v>
+        <v>SYLVIE GIGUÈRE,</v>
       </c>
       <c r="C10" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M10" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521047/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30945/index.do</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B11" t="str">
-        <v>CANADIAN WESTERN TRUST COMPANY</v>
+        <v>JOHN MCEWEN,</v>
       </c>
       <c r="C11" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M11" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521057/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30690/index.do</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v xml:space="preserve"> Susan Wong</v>
+        <v xml:space="preserve"> F.J. Pizzitelli</v>
       </c>
       <c r="B12" t="str">
-        <v>BUHLER VERSATILE INC.,</v>
+        <v>MARK TWOMEY,</v>
       </c>
       <c r="C12" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M12" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521046/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30938/index.do</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v xml:space="preserve"> Jean Marc Gagnon</v>
+        <v xml:space="preserve"> B. Paris</v>
       </c>
       <c r="B13" t="str">
-        <v>MARK ANDREWS,</v>
+        <v>HARVEY CHADWICK,</v>
       </c>
       <c r="C13" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M13" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521048/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30939/index.do</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v xml:space="preserve"> Jean Marc Gagnon</v>
+        <v xml:space="preserve"> Réal Favreau</v>
       </c>
       <c r="B14" t="str">
-        <v>MONIQUE GROULX,</v>
+        <v>LAIRD STEVENS,</v>
       </c>
       <c r="C14" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M14" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521049/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30961/index.do</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v xml:space="preserve"> Joanna Hill</v>
+        <v>Diane Campbell</v>
       </c>
       <c r="B15" t="str">
-        <v>VIVIANA RESER,</v>
+        <v>ROBERT ELWOOD,</v>
       </c>
       <c r="C15" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M15" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521058/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30950/index.do</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v>Valerie Miller</v>
       </c>
       <c r="B16" t="str">
-        <v>K&amp;D LOGGING LTD.,</v>
+        <v>GEORGE J. BRAKE,</v>
       </c>
       <c r="C16" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M16" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521055/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30947/index.do</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v xml:space="preserve"> Dominique Lafleur</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B17" t="str">
-        <v>1048547 ONTARIO INC.,</v>
+        <v>TERESA BRUNO,</v>
       </c>
       <c r="C17" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M17" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521059/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30943/index.do</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v xml:space="preserve"> Patrick Boyle</v>
+        <v>Valerie Miller</v>
       </c>
       <c r="B18" t="str">
-        <v>TONY DOUSSOT,</v>
+        <v>OSWALD F. ROBERTS,</v>
       </c>
       <c r="C18" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M18" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521064/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30948/index.do</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Justice G. Renaud</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B19" t="str">
-        <v>HEIDI MELENCHUK,</v>
+        <v>MOHAMMED RAHMAN,</v>
       </c>
       <c r="C19" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M19" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521072/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30949/index.do</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> Patrick Boyle</v>
       </c>
       <c r="B20" t="str">
-        <v>MARLENE ENNS,</v>
+        <v>MARGARET SWAIN,</v>
       </c>
       <c r="C20" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M20" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521065/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30979/index.do</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v xml:space="preserve"> Henry A. Visser</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B21" t="str">
-        <v>DAVID GOLDHAR,</v>
+        <v>9098-9005 QUEBEC INC.,</v>
       </c>
       <c r="C21" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M21" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521061/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30971/index.do</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v xml:space="preserve"> Monica Biringer</v>
+        <v xml:space="preserve"> Valerie Miller</v>
       </c>
       <c r="B22" t="str">
-        <v>JOSE ANTONIO VIRITO REYES,</v>
+        <v>KATHRYN KOSSOW,</v>
       </c>
       <c r="C22" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M22" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521120/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30953/index.do</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v xml:space="preserve"> Robert J. Hogan</v>
+        <v>F.J. Pizzitelli</v>
       </c>
       <c r="B23" t="str">
-        <v>ALL SPORTS MARKETING INC.,</v>
+        <v>REYNOLD DICKIE,</v>
       </c>
       <c r="C23" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M23" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521063/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30959/index.do</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v>Diane Campbell</v>
       </c>
       <c r="B24" t="str">
-        <v>BRUNO OLIVEIRA,</v>
+        <v>LAWRENCE WATTS, ELIZABETH BROCCOLI, VINTON MURRAY and ALFRED J.R. ADJETY,</v>
       </c>
       <c r="C24" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M24" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521067/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30955/index.do</v>
       </c>
     </row>
     <row r="25">
@@ -770,634 +770,1964 @@
         <v xml:space="preserve"> Patrick Boyle</v>
       </c>
       <c r="B25" t="str">
-        <v>CANADIAN SECURITY &amp;</v>
+        <v>SHIRLEY PATRICIA MCKENZIE,</v>
       </c>
       <c r="C25" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M25" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521066/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30983/index.do</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v xml:space="preserve"> Gabrielle St-Hilaire</v>
+        <v xml:space="preserve"> Valerie Miller</v>
       </c>
       <c r="B26" t="str">
-        <v>3792391 CANADA INC.,</v>
+        <v>WILLIAM A. LAWRENCE,</v>
       </c>
       <c r="C26" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M26" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521069/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30954/index.do</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v xml:space="preserve"> Dominique Lafleur</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B27" t="str">
-        <v>ANNA WAI MAN WAN,</v>
+        <v>YVONNE TUCK,</v>
       </c>
       <c r="C27" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M27" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521071/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30956/index.do</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v xml:space="preserve"> Ronald MacPhee</v>
+        <v xml:space="preserve"> Steven K. D'Arcy</v>
       </c>
       <c r="B28" t="str">
-        <v>A-SUPREME NURSING &amp; HOME CARE SERVICES INC.,</v>
+        <v>LANCE ANDERSON,</v>
       </c>
       <c r="C28" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M28" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521070/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30960/index.do</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v xml:space="preserve"> Monica Biringer</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B29" t="str">
-        <v>ALYKHAN HABIB HIRJEE,</v>
+        <v>DARLENE ANTHONY,</v>
       </c>
       <c r="C29" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M29" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521078/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30957/index.do</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B30" t="str">
-        <v>CO-OPERATIVE HAIL INSURANCE COMPANY LIMITED,</v>
+        <v>BRADMAN LEE,</v>
       </c>
       <c r="C30" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M30" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521074/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30958/index.do</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v xml:space="preserve"> Steven K. D’Arcy</v>
+        <v>Chief Judge Gerald J. Rip</v>
       </c>
       <c r="B31" t="str">
-        <v>THE BELL TELEPHONE COMPANY OF CANADA</v>
+        <v>DANIEL MARCOTTE,</v>
       </c>
       <c r="C31" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M31" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521075/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30963/index.do</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v xml:space="preserve"> Robert J. Hogan</v>
+        <v>Mr. Justice Randall Bocock</v>
       </c>
       <c r="B32" t="str">
-        <v>LUCY LITTLE,</v>
+        <v>RONALD SYDNEY PHILLIPS,</v>
       </c>
       <c r="C32" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M32" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521076/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30964/index.do</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v xml:space="preserve"> Joanna Hill</v>
+        <v>Mr. Justice Randall Bocock</v>
       </c>
       <c r="B33" t="str">
-        <v>JONATHON S. BREEN,</v>
+        <v>VIKRAM NANDAKUMAR,</v>
       </c>
       <c r="C33" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M33" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521079/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30965/index.do</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v xml:space="preserve"> Don R. Sommerfeldt</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B34" t="str">
-        <v>IRVING EBERT,</v>
+        <v>PIERRE LABRECQUE,</v>
       </c>
       <c r="C34" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M34" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521082/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30986/index.do</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v xml:space="preserve"> Jean Marc Gagnon</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B35" t="str">
-        <v>G DEWAR LAING,</v>
+        <v>CLÉMENT GIROUX,</v>
       </c>
       <c r="C35" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M35" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521081/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30966/index.do</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B36" t="str">
-        <v>EMMANUEL AZZOPARDI,</v>
+        <v>MARTIN PERRON,</v>
       </c>
       <c r="C36" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M36" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521092/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30967/index.do</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B37" t="str">
-        <v>SEAN O'HAGAN,</v>
+        <v>RÉAL BOUDREAU,</v>
       </c>
       <c r="C37" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M37" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521083/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30969/index.do</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v xml:space="preserve"> Don R. Sommerfeldt</v>
+        <v xml:space="preserve"> Paul Bédard</v>
       </c>
       <c r="B38" t="str">
-        <v>0808498 BC LTD.,</v>
+        <v>SÉBASTIEN GIRARD (PRO GESTION 3000),</v>
       </c>
       <c r="C38" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M38" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521087/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30970/index.do</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v xml:space="preserve"> Don R. Sommerfeldt</v>
+        <v xml:space="preserve"> B. Paris</v>
       </c>
       <c r="B39" t="str">
-        <v>ADELINA SIMONETTA,</v>
+        <v>CARLO MASSICOLLI,</v>
       </c>
       <c r="C39" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M39" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521090/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30973/index.do</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v xml:space="preserve"> Jean Marc Gagnon</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B40" t="str">
-        <v>SOUAD HAMMOUD,</v>
+        <v>BALBIR KAUR BASI,</v>
       </c>
       <c r="C40" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M40" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521089/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30976/index.do</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Gaston Jorré, Deputy Judge</v>
+        <v xml:space="preserve"> J.E. Hershfield</v>
       </c>
       <c r="B41" t="str">
-        <v>NEWFOUNDLAND BROADCASTING COMPANY LIMITED,</v>
+        <v>SURREY CITY CENTRE MALL LTD.,</v>
       </c>
       <c r="C41" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M41" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521086/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30975/index.do</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B42" t="str">
-        <v>2405124 ONTARIO LTD.,</v>
+        <v>DOUGLAS JOHN SUTCLIFFE,</v>
       </c>
       <c r="C42" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M42" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521085/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30974/index.do</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v xml:space="preserve"> David E. Graham</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B43" t="str">
-        <v>WINDSOR ELMS VILLAGE FOR CONTINUING CARE SOCIETY,</v>
+        <v>SALVATORE PERAGINE,</v>
       </c>
       <c r="C43" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M43" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521084/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30977/index.do</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v xml:space="preserve"> Gabrielle St-Hilaire</v>
+        <v xml:space="preserve"> Réal Favreau</v>
       </c>
       <c r="B44" t="str">
-        <v>MF ELECTRIC INCORPORATED,</v>
+        <v>AMY LE,</v>
       </c>
       <c r="C44" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M44" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521088/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30990/index.do</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v xml:space="preserve"> Sylvain Ouimet</v>
+        <v>Gaston Jorré</v>
       </c>
       <c r="B45" t="str">
-        <v>KEVIN LEE HACHULLA,</v>
+        <v>SARUP KUNDI,</v>
       </c>
       <c r="C45" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M45" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521100/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30678/index.do</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v xml:space="preserve"> Joanna Hill</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B46" t="str">
-        <v>ALLAN WERSTEIN,</v>
+        <v>VICKI ANNE WELCH,</v>
       </c>
       <c r="C46" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M46" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521093/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30978/index.do</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v xml:space="preserve"> Susan Wong</v>
+        <v xml:space="preserve"> Johanne D'Auray</v>
       </c>
       <c r="B47" t="str">
-        <v>PROSPERA CREDIT UNION,</v>
+        <v>MOTECH MOLDING INC. / MOTECH</v>
       </c>
       <c r="C47" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M47" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521091/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30982/index.do</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>David E. Graham</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B48" t="str">
-        <v>THE ESTATE OF VENENCE COTE,</v>
+        <v>GEOFFREY LAST,</v>
       </c>
       <c r="C48" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M48" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521094/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30980/index.do</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v xml:space="preserve"> Ronald MacPhee</v>
+        <v xml:space="preserve"> Patrick Boyle</v>
       </c>
       <c r="B49" t="str">
-        <v>GARG INVESTMENTS INC.,</v>
+        <v>SUZANNE ASHTON</v>
       </c>
       <c r="C49" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M49" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521097/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30981/index.do</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v xml:space="preserve"> Joanna Hill</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B50" t="str">
-        <v>DARREN JAMIESON,</v>
+        <v>STANISLAW PAWLAK, JADWIGA PAWLAK,</v>
       </c>
       <c r="C50" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M50" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521098/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30987/index.do</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>David E. Graham</v>
+        <v xml:space="preserve"> Patrick Boyle</v>
       </c>
       <c r="B51" t="str">
-        <v>BRANDON OSADCHUK,</v>
+        <v>SPRUCE CREDIT UNION,</v>
       </c>
       <c r="C51" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M51" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521096/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30984/index.do</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v xml:space="preserve"> Dominique Lafleur</v>
+        <v>Mr. Justice Randall Bocock</v>
       </c>
       <c r="B52" t="str">
-        <v>HILLCORE FINANCIAL CORPORATION,</v>
+        <v>THE BRENT KERN FAMILY TRUST,</v>
       </c>
       <c r="C52" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M52" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521099/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30993/index.do</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Mr. Justice Randall S. Bocock</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B53" t="str">
-        <v>THE UNIVERSITY OF NEW BRUNSWICK,</v>
+        <v>COLIN FOREMAN,</v>
       </c>
       <c r="C53" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M53" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521101/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30689/index.do</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v xml:space="preserve"> Don R. Sommerfeldt</v>
+        <v>B. Paris</v>
       </c>
       <c r="B54" t="str">
-        <v>S. ROBERT CHAD,</v>
+        <v>OBARO OKOROZE,</v>
       </c>
       <c r="C54" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M54" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521102/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30991/index.do</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v>Alain Tardif</v>
       </c>
       <c r="B55" t="str">
-        <v>YIN LI,</v>
+        <v>BOISSONNEAULT GROUPE IMMOBILIER INC.,</v>
       </c>
       <c r="C55" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M55" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521106/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30988/index.do</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v xml:space="preserve"> Sylvain Ouimet</v>
+        <v xml:space="preserve"> Wyman W. Webb</v>
       </c>
       <c r="B56" t="str">
-        <v>JOHN DOE[*],</v>
+        <v>MICHELLE CAMPBELL,</v>
       </c>
       <c r="C56" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M56" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521111/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30995/index.do</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v xml:space="preserve"> Susan Wong</v>
+        <v xml:space="preserve"> Pierre Archambault</v>
       </c>
       <c r="B57" t="str">
-        <v>JANIS ROBB,</v>
+        <v>9101-2310 QUÉBEC INC.,</v>
       </c>
       <c r="C57" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M57" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521104/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30997/index.do</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Justice Gaston Jorré</v>
+        <v xml:space="preserve"> Alain Tardif</v>
       </c>
       <c r="B58" t="str">
-        <v>OM GUPTA,</v>
+        <v>LABORATOIRE DU-VAR INC.,</v>
       </c>
       <c r="C58" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M58" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521108/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30994/index.do</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v xml:space="preserve"> Monica Biringer</v>
+        <v xml:space="preserve"> Alain Tardif</v>
       </c>
       <c r="B59" t="str">
-        <v>RODERIC PARKER,</v>
+        <v>DANIELLE LEMIRE,</v>
       </c>
       <c r="C59" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M59" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521109/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30992/index.do</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> Réal Favreau</v>
       </c>
       <c r="B60" t="str">
-        <v>MARIA BALATONI,</v>
+        <v>SUNNY LYTLE,</v>
       </c>
       <c r="C60" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M60" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521124/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31036/index.do</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B61" t="str">
-        <v>JEFFREY P ADAMS,</v>
+        <v>NORTH DELTA REAL HOT YOGA LTD.,</v>
       </c>
       <c r="C61" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M61" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521113/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31071/index.do</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v xml:space="preserve"> Bruce Russell</v>
+        <v xml:space="preserve"> Alain Tardif</v>
       </c>
       <c r="B62" t="str">
-        <v>GREGORY A. GESSNER,</v>
+        <v>MARTIAL MORISSETTE,</v>
       </c>
       <c r="C62" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M62" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521112/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30705/index.do</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Mr. Justice Randall S. Bocock</v>
+        <v xml:space="preserve"> J.M. Woods</v>
       </c>
       <c r="B63" t="str">
-        <v>ALEXANDRE PAPOUCHINE,</v>
+        <v>ANA C. DEAN, o/a ANA’S CARE &amp; HOME SUPPORT,</v>
       </c>
       <c r="C63" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M63" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521116/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30998/index.do</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v xml:space="preserve"> Gabrielle St-Hilaire</v>
+        <v xml:space="preserve"> Réal Favreau</v>
       </c>
       <c r="B64" t="str">
-        <v>SOPHIE PAYETTE,</v>
+        <v>HASSAN YAZDANI,</v>
       </c>
       <c r="C64" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M64" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521040/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30996/index.do</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v xml:space="preserve"> Sylvain Ouimet</v>
+        <v xml:space="preserve"> Campbell J. Miller</v>
       </c>
       <c r="B65" t="str">
-        <v>JOHN DOE[*],</v>
+        <v>KEVIN D'AMORE,</v>
       </c>
       <c r="C65" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M65" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521114/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31000/index.do</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v xml:space="preserve"> Robert J. Hogan</v>
+        <v xml:space="preserve"> Lucie Lamarre</v>
       </c>
       <c r="B66" t="str">
-        <v>AMEX BANK OF CANADA,</v>
+        <v>FRANCE MARTEL,</v>
       </c>
       <c r="C66" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M66" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521117/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31001/index.do</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v xml:space="preserve"> David E. Spiro</v>
+        <v xml:space="preserve"> T.E. Margeson</v>
       </c>
       <c r="B67" t="str">
-        <v>AFB JANITORIAL SERVICES INC.,</v>
+        <v>TRANSALTA CORPORATION,</v>
       </c>
       <c r="C67" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M67" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521119/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30999/index.do</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Steven K. D’Arcy</v>
+        <v xml:space="preserve"> Robert J. Hogan</v>
       </c>
       <c r="B68" t="str">
-        <v>MARINE ATLANTIC INC.,</v>
+        <v>1726437 ONTARIO INC. o/a</v>
       </c>
       <c r="C68" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M68" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521122/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31003/index.do</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Mr. Justice Randall S. Bocock</v>
+        <v xml:space="preserve"> Robert J. Hogan</v>
       </c>
       <c r="B69" t="str">
-        <v>CLARE OSBORNE,</v>
+        <v>SWS COMMUNICATION INC.,</v>
       </c>
       <c r="C69" t="str">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="M69" t="str">
-        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/521123/index.do</v>
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31002/index.do</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v xml:space="preserve"> Campbell J. Miller</v>
+      </c>
+      <c r="B70" t="str">
+        <v>JULIE BURKE,</v>
+      </c>
+      <c r="C70" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M70" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31005/index.do</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v xml:space="preserve"> Valerie Miller</v>
+      </c>
+      <c r="B71" t="str">
+        <v>JUDITH MACLEOD,</v>
+      </c>
+      <c r="C71" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M71" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31006/index.do</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v xml:space="preserve">JudgeName Not Found in Pattern also </v>
+      </c>
+      <c r="B72" t="str">
+        <v>JUDY LEQUIER,</v>
+      </c>
+      <c r="C72" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M72" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31007/index.do</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Jean-Louis Batiot</v>
+      </c>
+      <c r="B73" t="str">
+        <v>CHARLES TOUPIN,</v>
+      </c>
+      <c r="C73" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M73" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31012/index.do</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Mr. Justice Randall Bocock</v>
+      </c>
+      <c r="B74" t="str">
+        <v>RENATE BRAUER,</v>
+      </c>
+      <c r="C74" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M74" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31008/index.do</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Mr. Justice Randall Bocock</v>
+      </c>
+      <c r="B75" t="str">
+        <v>YOUNG TILE INC.,</v>
+      </c>
+      <c r="C75" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M75" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31009/index.do</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B76" t="str">
+        <v>ALINE LÉVESQUE,</v>
+      </c>
+      <c r="C76" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M76" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31011/index.do</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B77" t="str">
+        <v>SUCCESSION OF SUZIE BROUSSEAU,</v>
+      </c>
+      <c r="C77" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M77" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31010/index.do</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v xml:space="preserve"> B. Paris</v>
+      </c>
+      <c r="B78" t="str">
+        <v>MAWUEWO K.J. AFOVIA,</v>
+      </c>
+      <c r="C78" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M78" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31013/index.do</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v xml:space="preserve"> Diane Campbell</v>
+      </c>
+      <c r="B79" t="str">
+        <v>SURINDER HAYER,</v>
+      </c>
+      <c r="C79" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M79" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31015/index.do</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B80" t="str">
+        <v>MAC'S CONVENIENCE STORES INC.,</v>
+      </c>
+      <c r="C80" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M80" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31016/index.do</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B81" t="str">
+        <v>BILL JORDAN,</v>
+      </c>
+      <c r="C81" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M81" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31014/index.do</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v xml:space="preserve"> Jean-Louis Batiot</v>
+      </c>
+      <c r="B82" t="str">
+        <v>LES CONSTRUCTIONS MARABELLA INC.,</v>
+      </c>
+      <c r="C82" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M82" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31020/index.do</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B83" t="str">
+        <v>WALFRED ERICKSON,</v>
+      </c>
+      <c r="C83" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M83" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31017/index.do</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v xml:space="preserve"> Réal Favreau</v>
+      </c>
+      <c r="B84" t="str">
+        <v>1259066 ONTARIO LIMITED,</v>
+      </c>
+      <c r="C84" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M84" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31028/index.do</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B85" t="str">
+        <v>INTEGRANUITY MARKETING LTD.,</v>
+      </c>
+      <c r="C85" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M85" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30653/index.do</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v xml:space="preserve"> Gaston Jorré</v>
+      </c>
+      <c r="B86" t="str">
+        <v>HÉLÈNE L. PERRON,</v>
+      </c>
+      <c r="C86" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M86" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30691/index.do</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B87" t="str">
+        <v>9134-2485 QUEBEC INC.,</v>
+      </c>
+      <c r="C87" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M87" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31019/index.do</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B88" t="str">
+        <v>ALEXANDER TRAN,</v>
+      </c>
+      <c r="C88" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M88" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31021/index.do</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>B. Paris</v>
+      </c>
+      <c r="B89" t="str">
+        <v>MICHAEL PALANGIO,</v>
+      </c>
+      <c r="C89" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M89" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31022/index.do</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Mr. Justice Randall Bocock</v>
+      </c>
+      <c r="B90" t="str">
+        <v>ALLEN BERG,</v>
+      </c>
+      <c r="C90" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M90" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31023/index.do</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Gaston Jorré</v>
+      </c>
+      <c r="B91" t="str">
+        <v>TERASEN INTERNATIONAL INC.</v>
+      </c>
+      <c r="C91" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M91" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31054/index.do</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v xml:space="preserve"> Valerie Miller</v>
+      </c>
+      <c r="B92" t="str">
+        <v>THE ESTATE OF THE LATE ANNA NTAKOS,</v>
+      </c>
+      <c r="C92" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M92" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31024/index.do</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B93" t="str">
+        <v>MICHAEL E. DUKE,</v>
+      </c>
+      <c r="C93" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M93" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30694/index.do</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Chief Justice Gerald J. Rip</v>
+      </c>
+      <c r="B94" t="str">
+        <v>ÉCOLE DE LANGUES ABCE INC.,</v>
+      </c>
+      <c r="C94" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M94" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31025/index.do</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B95" t="str">
+        <v>GEORGIOS (GEORGE) PRIFTIS,</v>
+      </c>
+      <c r="C95" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M95" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31035/index.do</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B96" t="str">
+        <v>MARIE-CLAUDE POULIN,</v>
+      </c>
+      <c r="C96" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M96" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31032/index.do</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v xml:space="preserve"> Johanne D’Auray</v>
+      </c>
+      <c r="B97" t="str">
+        <v>CONSTRUCTION BIAGIO MAIORINO INC.,</v>
+      </c>
+      <c r="C97" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M97" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31026/index.do</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v xml:space="preserve"> Campbell J. Miller</v>
+      </c>
+      <c r="B98" t="str">
+        <v>OM P. MITTAL,</v>
+      </c>
+      <c r="C98" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M98" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31027/index.do</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B99" t="str">
+        <v>DARYL CHRISTENSEN,</v>
+      </c>
+      <c r="C99" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M99" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30695/index.do</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v xml:space="preserve"> Campbell J. Miller</v>
+      </c>
+      <c r="B100" t="str">
+        <v>NRT TECHNOLOGY CORP.,</v>
+      </c>
+      <c r="C100" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M100" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31030/index.do</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B101" t="str">
+        <v>DALI BENTOLILA,</v>
+      </c>
+      <c r="C101" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M101" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31033/index.do</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B102" t="str">
+        <v>830480 ALBERTA INC.,</v>
+      </c>
+      <c r="C102" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M102" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31031/index.do</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>Rommel G. Masse</v>
+      </c>
+      <c r="B103" t="str">
+        <v>CHANTAL CONSTANTIN,</v>
+      </c>
+      <c r="C103" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M103" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31078/index.do</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B104" t="str">
+        <v>LAURIANNE GAUCHER,</v>
+      </c>
+      <c r="C104" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M104" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30696/index.do</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v xml:space="preserve"> Valerie Miller</v>
+      </c>
+      <c r="B105" t="str">
+        <v>FIONA J. EDWARDS,</v>
+      </c>
+      <c r="C105" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M105" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31034/index.do</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v xml:space="preserve"> B. Paris</v>
+      </c>
+      <c r="B106" t="str">
+        <v>NORAN WEST DEVELOPMENTS LTD.,</v>
+      </c>
+      <c r="C106" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M106" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31038/index.do</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B107" t="str">
+        <v>DARLENE STEWART,</v>
+      </c>
+      <c r="C107" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M107" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31037/index.do</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B108" t="str">
+        <v>ALGONQUIN LANDSCAPING LTD.,</v>
+      </c>
+      <c r="C108" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M108" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31039/index.do</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v xml:space="preserve"> Gaston Jorré</v>
+      </c>
+      <c r="B109" t="str">
+        <v>SYNER/PLUS INC.,</v>
+      </c>
+      <c r="C109" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M109" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30697/index.do</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B110" t="str">
+        <v>KARL KRATOCHWIL,</v>
+      </c>
+      <c r="C110" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M110" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30698/index.do</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v xml:space="preserve"> Campbell J. Miller</v>
+      </c>
+      <c r="B111" t="str">
+        <v>IAN BROWN,</v>
+      </c>
+      <c r="C111" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M111" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31043/index.do</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v xml:space="preserve"> Patrick Boyle</v>
+      </c>
+      <c r="B112" t="str">
+        <v>BRENDA WALKOWIAK,</v>
+      </c>
+      <c r="C112" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M112" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31044/index.do</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B113" t="str">
+        <v>JOHN E. KUCH,</v>
+      </c>
+      <c r="C113" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M113" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31045/index.do</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v xml:space="preserve"> Steven K. D’Arcy</v>
+      </c>
+      <c r="B114" t="str">
+        <v>ELENA SHULKOV,</v>
+      </c>
+      <c r="C114" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M114" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31046/index.do</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v xml:space="preserve"> Patrick Boyle</v>
+      </c>
+      <c r="B115" t="str">
+        <v>MARGARET SWAIN,</v>
+      </c>
+      <c r="C115" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M115" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30701/index.do</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v xml:space="preserve"> Gaston Jorré</v>
+      </c>
+      <c r="B116" t="str">
+        <v>2868-3977 QUÉBEC INC.,</v>
+      </c>
+      <c r="C116" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M116" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30700/index.do</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v xml:space="preserve"> Wyman W. Webb</v>
+      </c>
+      <c r="B117" t="str">
+        <v>JO-ANN NADALIN,</v>
+      </c>
+      <c r="C117" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M117" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30703/index.do</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B118" t="str">
+        <v>TEHSEEN FATIMA,</v>
+      </c>
+      <c r="C118" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M118" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30699/index.do</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B119" t="str">
+        <v>GIFFORD H. TOOLE,</v>
+      </c>
+      <c r="C119" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M119" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30702/index.do</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B120" t="str">
+        <v>JAMES O. GROSSETT,</v>
+      </c>
+      <c r="C120" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M120" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30710/index.do</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B121" t="str">
+        <v>VIDA BRUCE,</v>
+      </c>
+      <c r="C121" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M121" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30704/index.do</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v xml:space="preserve"> Johanne D’Auray</v>
+      </c>
+      <c r="B122" t="str">
+        <v>JACQUES POISSON,</v>
+      </c>
+      <c r="C122" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M122" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30713/index.do</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B123" t="str">
+        <v>DAVID LAM,</v>
+      </c>
+      <c r="C123" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M123" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30708/index.do</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v xml:space="preserve"> Patrick Boyle</v>
+      </c>
+      <c r="B124" t="str">
+        <v>MORGUARD CORPORATION,</v>
+      </c>
+      <c r="C124" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M124" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30725/index.do</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B125" t="str">
+        <v>AZIZULLAH HAFIZY,</v>
+      </c>
+      <c r="C125" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M125" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30709/index.do</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v xml:space="preserve">JudgeName Not Found in Pattern also </v>
+      </c>
+      <c r="B126" t="str">
+        <v>VELCRO CANADA INC.,</v>
+      </c>
+      <c r="C126" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M126" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30726/index.do</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v xml:space="preserve"> Valerie Miller</v>
+      </c>
+      <c r="B127" t="str">
+        <v>DOLORES ROMANUK,</v>
+      </c>
+      <c r="C127" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M127" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30714/index.do</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B128" t="str">
+        <v>RAYMOND F. WAGNER,</v>
+      </c>
+      <c r="C128" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M128" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30715/index.do</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Nathalie Dion, exECUTOR</v>
+      </c>
+      <c r="C129" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M129" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30658/index.do</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>N. Weisman</v>
+      </c>
+      <c r="B130" t="str">
+        <v>PRO-PHARMA CONTRACT SELLING SERVICES INC.,</v>
+      </c>
+      <c r="C130" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M130" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30728/index.do</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v xml:space="preserve"> Wyman W. Webb</v>
+      </c>
+      <c r="B131" t="str">
+        <v>CARL CURRIE,</v>
+      </c>
+      <c r="C131" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M131" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30736/index.do</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v xml:space="preserve"> Gaston Jorré</v>
+      </c>
+      <c r="B132" t="str">
+        <v>THÉRÈSE DESGAGNÉ,</v>
+      </c>
+      <c r="C132" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M132" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30724/index.do</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B133" t="str">
+        <v>MICHAEL J. BARKER,</v>
+      </c>
+      <c r="C133" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M133" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30730/index.do</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B134" t="str">
+        <v>MARY KELLY,</v>
+      </c>
+      <c r="C134" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M134" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30731/index.do</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v xml:space="preserve"> Johanne D'Auray</v>
+      </c>
+      <c r="B135" t="str">
+        <v>DANIEL RHEAUME,</v>
+      </c>
+      <c r="C135" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M135" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30733/index.do</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v xml:space="preserve"> Gaston Jorré</v>
+      </c>
+      <c r="B136" t="str">
+        <v>CALGARY BOARD OF EDUCATION,</v>
+      </c>
+      <c r="C136" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M136" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30677/index.do</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B137" t="str">
+        <v>M.A.P. (Mentorship, Aftercare, Presence),</v>
+      </c>
+      <c r="C137" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M137" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30734/index.do</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v xml:space="preserve"> Réal Favreau</v>
+      </c>
+      <c r="B138" t="str">
+        <v>KHEDIDJA MESSAR-SPLINTER,</v>
+      </c>
+      <c r="C138" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M138" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30740/index.do</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B139" t="str">
+        <v>BRUCE W. DOUGLAS,</v>
+      </c>
+      <c r="C139" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M139" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30735/index.do</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v xml:space="preserve"> Wyman W. Webb</v>
+      </c>
+      <c r="B140" t="str">
+        <v>RHETT LARSEN,</v>
+      </c>
+      <c r="C140" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M140" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30738/index.do</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B141" t="str">
+        <v>JEAN-GUY MALO,</v>
+      </c>
+      <c r="C141" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M141" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30739/index.do</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v xml:space="preserve"> Robert J. Hogan</v>
+      </c>
+      <c r="B142" t="str">
+        <v>GALINA MILOVA,</v>
+      </c>
+      <c r="C142" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M142" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30742/index.do</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>Réal Favreau</v>
+      </c>
+      <c r="B143" t="str">
+        <v>JOSÉE OUELLET,</v>
+      </c>
+      <c r="C143" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M143" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30745/index.do</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B144" t="str">
+        <v>BELINDA J. SNOW,</v>
+      </c>
+      <c r="C144" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M144" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30741/index.do</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v xml:space="preserve"> T.E. Margeson</v>
+      </c>
+      <c r="B145" t="str">
+        <v>ALLAN McLARTY,</v>
+      </c>
+      <c r="C145" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M145" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30744/index.do</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v xml:space="preserve"> Réal Favreau</v>
+      </c>
+      <c r="B146" t="str">
+        <v>FRED WAGNER,</v>
+      </c>
+      <c r="C146" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M146" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30912/index.do</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B147" t="str">
+        <v>McCLARTY FAMILY TRUST,</v>
+      </c>
+      <c r="C147" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M147" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30858/index.do</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B148" t="str">
+        <v>EN HUANG,</v>
+      </c>
+      <c r="C148" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M148" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30743/index.do</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B149" t="str">
+        <v>DIANE JACQUES,</v>
+      </c>
+      <c r="C149" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M149" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30755/index.do</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B150" t="str">
+        <v>NICOLAS AKOURI,</v>
+      </c>
+      <c r="C150" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M150" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30746/index.do</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v xml:space="preserve"> Patrick Boyle</v>
+      </c>
+      <c r="B151" t="str">
+        <v>SAMIPAL DHALIWAL,</v>
+      </c>
+      <c r="C151" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M151" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30749/index.do</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B152" t="str">
+        <v>ZENON KEDZIERSKI,</v>
+      </c>
+      <c r="C152" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M152" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30747/index.do</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v xml:space="preserve"> T.E. Margeson</v>
+      </c>
+      <c r="B153" t="str">
+        <v>TRANSALTA CORPORATION,</v>
+      </c>
+      <c r="C153" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M153" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30748/index.do</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v xml:space="preserve"> Paul Bédard</v>
+      </c>
+      <c r="B154" t="str">
+        <v>LAVIN ASSOCIÉS INC,</v>
+      </c>
+      <c r="C154" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M154" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30827/index.do</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v xml:space="preserve"> François Angers</v>
+      </c>
+      <c r="B155" t="str">
+        <v>LEAH DIOME,</v>
+      </c>
+      <c r="C155" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M155" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30707/index.do</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B156" t="str">
+        <v>george trieste,</v>
+      </c>
+      <c r="C156" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M156" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30753/index.do</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v xml:space="preserve"> Lucie Lamarre</v>
+      </c>
+      <c r="B157" t="str">
+        <v>Samir Sarophim,</v>
+      </c>
+      <c r="C157" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M157" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30752/index.do</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v xml:space="preserve"> Réal Favreau</v>
+      </c>
+      <c r="B158" t="str">
+        <v>DANIEL BÉLANGER,</v>
+      </c>
+      <c r="C158" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M158" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30772/index.do</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v xml:space="preserve">JudgeName Not Found in Pattern also </v>
+      </c>
+      <c r="B159" t="str">
+        <v>ANDRÉ DROUIN,</v>
+      </c>
+      <c r="C159" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M159" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30751/index.do</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v xml:space="preserve"> Patrick Boyle</v>
+      </c>
+      <c r="B160" t="str">
+        <v>MATTHEW J. VEGH,</v>
+      </c>
+      <c r="C160" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M160" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30765/index.do</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v xml:space="preserve"> J.M. Woods</v>
+      </c>
+      <c r="B161" t="str">
+        <v>SHIRAZ VIRANI,</v>
+      </c>
+      <c r="C161" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M161" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30754/index.do</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>Valerie Miller</v>
+      </c>
+      <c r="B162" t="str">
+        <v>ROANEX HOMES LTD.,</v>
+      </c>
+      <c r="C162" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M162" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30759/index.do</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v xml:space="preserve"> G. A. Sheridan</v>
+      </c>
+      <c r="B163" t="str">
+        <v>JAMES ZSEBOK,</v>
+      </c>
+      <c r="C163" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M163" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/30756/index.do</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>Mr. Justice Randall Bocock</v>
+      </c>
+      <c r="B164" t="str">
+        <v>1443900 ONT. INC.</v>
+      </c>
+      <c r="C164" t="str">
+        <v>2012</v>
+      </c>
+      <c r="M164" t="str">
+        <v>https://decision.tcc-cci.gc.ca/tcc-cci/decisions/en/item/31086/index.do</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M69"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M164"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>